<commit_message>
This commit includes the Admin and User flow
</commit_message>
<xml_diff>
--- a/DataSheet.xlsx
+++ b/DataSheet.xlsx
@@ -427,7 +427,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:B3"/>
+  <dimension ref="A1:B4"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="D8" sqref="D8"/>
@@ -466,6 +466,18 @@
         </is>
       </c>
       <c r="B3" t="inlineStr">
+        <is>
+          <t>1234</t>
+        </is>
+      </c>
+    </row>
+    <row r="4">
+      <c r="A4" t="inlineStr">
+        <is>
+          <t>sru</t>
+        </is>
+      </c>
+      <c r="B4" t="inlineStr">
         <is>
           <t>1234</t>
         </is>
@@ -1208,7 +1220,7 @@
         </is>
       </c>
       <c r="M2" t="n">
-        <v>20</v>
+        <v>18</v>
       </c>
       <c r="N2" t="n">
         <v>1</v>

</xml_diff>

<commit_message>
This commit involves solving this issue with cancel ticket issue
</commit_message>
<xml_diff>
--- a/DataSheet.xlsx
+++ b/DataSheet.xlsx
@@ -3,13 +3,12 @@
 <workbook xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <workbookPr/>
   <bookViews>
-    <workbookView visibility="visible" minimized="0" showHorizontalScroll="1" showVerticalScroll="1" showSheetTabs="1" xWindow="380" yWindow="500" windowWidth="28040" windowHeight="15820" tabRatio="600" firstSheet="0" activeTab="0" autoFilterDateGrouping="1"/>
+    <workbookView visibility="visible" minimized="0" showHorizontalScroll="1" showVerticalScroll="1" showSheetTabs="1" xWindow="380" yWindow="500" windowWidth="28040" windowHeight="15800" tabRatio="600" firstSheet="0" activeTab="1" autoFilterDateGrouping="1"/>
   </bookViews>
   <sheets>
     <sheet name="Details" sheetId="1" state="visible" r:id="rId1"/>
     <sheet name="Pushpa" sheetId="2" state="visible" r:id="rId2"/>
     <sheet name="Krish" sheetId="3" state="visible" r:id="rId3"/>
-    <sheet name="WALLE" sheetId="4" state="visible" r:id="rId4"/>
   </sheets>
   <definedNames/>
   <calcPr calcId="0" fullCalcOnLoad="1"/>
@@ -427,10 +426,10 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:B4"/>
+  <dimension ref="A1:B7"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D8" sqref="D8"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="D7" sqref="D7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16"/>
@@ -450,7 +449,7 @@
     <row r="2">
       <c r="A2" t="inlineStr">
         <is>
-          <t>sru</t>
+          <t>hasher</t>
         </is>
       </c>
       <c r="B2" t="inlineStr">
@@ -462,7 +461,7 @@
     <row r="3">
       <c r="A3" t="inlineStr">
         <is>
-          <t>vasa</t>
+          <t>test2</t>
         </is>
       </c>
       <c r="B3" t="inlineStr">
@@ -474,12 +473,48 @@
     <row r="4">
       <c r="A4" t="inlineStr">
         <is>
-          <t>sru</t>
+          <t>vasa</t>
         </is>
       </c>
       <c r="B4" t="inlineStr">
         <is>
           <t>1234</t>
+        </is>
+      </c>
+    </row>
+    <row r="5">
+      <c r="A5" t="inlineStr">
+        <is>
+          <t>vasa</t>
+        </is>
+      </c>
+      <c r="B5" t="inlineStr">
+        <is>
+          <t>123</t>
+        </is>
+      </c>
+    </row>
+    <row r="6">
+      <c r="A6" t="inlineStr">
+        <is>
+          <t>vasa</t>
+        </is>
+      </c>
+      <c r="B6" t="inlineStr">
+        <is>
+          <t>123</t>
+        </is>
+      </c>
+    </row>
+    <row r="7">
+      <c r="A7" t="inlineStr">
+        <is>
+          <t>jerry</t>
+        </is>
+      </c>
+      <c r="B7" t="inlineStr">
+        <is>
+          <t>123</t>
         </is>
       </c>
     </row>
@@ -496,8 +531,8 @@
   </sheetPr>
   <dimension ref="A1:N4"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A1" sqref="A1"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="M2" sqref="M2:M4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="16"/>
@@ -610,7 +645,7 @@
       </c>
       <c r="H2" t="inlineStr">
         <is>
-          <t>08:00-10:00</t>
+          <t>10:00-12:00</t>
         </is>
       </c>
       <c r="I2" t="inlineStr">
@@ -634,7 +669,7 @@
         </is>
       </c>
       <c r="M2" t="n">
-        <v>50</v>
+        <v>100</v>
       </c>
       <c r="N2" t="n">
         <v>2</v>
@@ -678,7 +713,7 @@
       </c>
       <c r="H3" t="inlineStr">
         <is>
-          <t>10:30-12:30</t>
+          <t>12:30-02:30</t>
         </is>
       </c>
       <c r="I3" t="inlineStr">
@@ -702,7 +737,7 @@
         </is>
       </c>
       <c r="M3" t="n">
-        <v>45</v>
+        <v>100</v>
       </c>
     </row>
     <row r="4">
@@ -743,7 +778,7 @@
       </c>
       <c r="H4" t="inlineStr">
         <is>
-          <t>1:00-03:00</t>
+          <t>03:00-05:00</t>
         </is>
       </c>
       <c r="I4" t="inlineStr">
@@ -766,10 +801,8 @@
           <t>30</t>
         </is>
       </c>
-      <c r="M4" t="inlineStr">
-        <is>
-          <t>50</t>
-        </is>
+      <c r="M4" t="n">
+        <v>100</v>
       </c>
     </row>
   </sheetData>
@@ -786,7 +819,7 @@
   <dimension ref="A1:N4"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A1" sqref="A1"/>
+      <selection activeCell="M11" sqref="M11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="16"/>
@@ -901,7 +934,7 @@
       </c>
       <c r="H2" t="inlineStr">
         <is>
-          <t>08:00-10:00</t>
+          <t>10:00-12:00</t>
         </is>
       </c>
       <c r="I2" t="inlineStr">
@@ -924,10 +957,8 @@
           <t>30</t>
         </is>
       </c>
-      <c r="M2" t="inlineStr">
-        <is>
-          <t>20</t>
-        </is>
+      <c r="M2" t="n">
+        <v>100</v>
       </c>
       <c r="N2" t="n">
         <v>1</v>
@@ -971,7 +1002,7 @@
       </c>
       <c r="H3" t="inlineStr">
         <is>
-          <t>10:30-12:30</t>
+          <t>12:30-02:30</t>
         </is>
       </c>
       <c r="I3" t="inlineStr">
@@ -994,10 +1025,8 @@
           <t>30</t>
         </is>
       </c>
-      <c r="M3" t="inlineStr">
-        <is>
-          <t>20</t>
-        </is>
+      <c r="M3" t="n">
+        <v>100</v>
       </c>
     </row>
     <row r="4">
@@ -1038,7 +1067,7 @@
       </c>
       <c r="H4" t="inlineStr">
         <is>
-          <t>1:00-03:00</t>
+          <t>03:00-05:00</t>
         </is>
       </c>
       <c r="I4" t="inlineStr">
@@ -1061,303 +1090,8 @@
           <t>30</t>
         </is>
       </c>
-      <c r="M4" t="inlineStr">
-        <is>
-          <t>20</t>
-        </is>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <sheetPr>
-    <outlinePr summaryBelow="1" summaryRight="1"/>
-    <pageSetUpPr/>
-  </sheetPr>
-  <dimension ref="A1:N4"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A1" sqref="A1"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="16"/>
-  <sheetData>
-    <row r="1">
-      <c r="A1" t="inlineStr">
-        <is>
-          <t>title</t>
-        </is>
-      </c>
-      <c r="B1" t="inlineStr">
-        <is>
-          <t>genre</t>
-        </is>
-      </c>
-      <c r="C1" t="inlineStr">
-        <is>
-          <t>length</t>
-        </is>
-      </c>
-      <c r="D1" t="inlineStr">
-        <is>
-          <t>cast</t>
-        </is>
-      </c>
-      <c r="E1" t="inlineStr">
-        <is>
-          <t>director</t>
-        </is>
-      </c>
-      <c r="F1" t="inlineStr">
-        <is>
-          <t>rating</t>
-        </is>
-      </c>
-      <c r="G1" t="inlineStr">
-        <is>
-          <t>language</t>
-        </is>
-      </c>
-      <c r="H1" t="inlineStr">
-        <is>
-          <t>timings</t>
-        </is>
-      </c>
-      <c r="I1" t="inlineStr">
-        <is>
-          <t>shows_per_day</t>
-        </is>
-      </c>
-      <c r="J1" t="inlineStr">
-        <is>
-          <t>firstshow</t>
-        </is>
-      </c>
-      <c r="K1" t="inlineStr">
-        <is>
-          <t>interval_time</t>
-        </is>
-      </c>
-      <c r="L1" t="inlineStr">
-        <is>
-          <t>gap</t>
-        </is>
-      </c>
-      <c r="M1" t="inlineStr">
-        <is>
-          <t>capacity</t>
-        </is>
-      </c>
-      <c r="N1" t="inlineStr">
-        <is>
-          <t>user_count</t>
-        </is>
-      </c>
-    </row>
-    <row r="2">
-      <c r="A2" t="inlineStr">
-        <is>
-          <t>WALLE</t>
-        </is>
-      </c>
-      <c r="B2" t="inlineStr">
-        <is>
-          <t>comedy</t>
-        </is>
-      </c>
-      <c r="C2" t="inlineStr">
-        <is>
-          <t>120</t>
-        </is>
-      </c>
-      <c r="D2" t="inlineStr">
-        <is>
-          <t>robots</t>
-        </is>
-      </c>
-      <c r="E2" t="inlineStr">
-        <is>
-          <t>eva</t>
-        </is>
-      </c>
-      <c r="F2" t="inlineStr">
-        <is>
-          <t>5</t>
-        </is>
-      </c>
-      <c r="G2" t="inlineStr">
-        <is>
-          <t>English</t>
-        </is>
-      </c>
-      <c r="H2" t="inlineStr">
-        <is>
-          <t>10:00-12:00</t>
-        </is>
-      </c>
-      <c r="I2" t="inlineStr">
-        <is>
-          <t>3</t>
-        </is>
-      </c>
-      <c r="J2" t="inlineStr">
-        <is>
-          <t>8</t>
-        </is>
-      </c>
-      <c r="K2" t="inlineStr">
-        <is>
-          <t>15</t>
-        </is>
-      </c>
-      <c r="L2" t="inlineStr">
-        <is>
-          <t>15</t>
-        </is>
-      </c>
-      <c r="M2" t="n">
-        <v>18</v>
-      </c>
-      <c r="N2" t="n">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="3">
-      <c r="A3" t="inlineStr">
-        <is>
-          <t>WALLE</t>
-        </is>
-      </c>
-      <c r="B3" t="inlineStr">
-        <is>
-          <t>comedy</t>
-        </is>
-      </c>
-      <c r="C3" t="inlineStr">
-        <is>
-          <t>120</t>
-        </is>
-      </c>
-      <c r="D3" t="inlineStr">
-        <is>
-          <t>robots</t>
-        </is>
-      </c>
-      <c r="E3" t="inlineStr">
-        <is>
-          <t>eva</t>
-        </is>
-      </c>
-      <c r="F3" t="inlineStr">
-        <is>
-          <t>5</t>
-        </is>
-      </c>
-      <c r="G3" t="inlineStr">
-        <is>
-          <t>English</t>
-        </is>
-      </c>
-      <c r="H3" t="inlineStr">
-        <is>
-          <t>12:30-02:30</t>
-        </is>
-      </c>
-      <c r="I3" t="inlineStr">
-        <is>
-          <t>3</t>
-        </is>
-      </c>
-      <c r="J3" t="inlineStr">
-        <is>
-          <t>8</t>
-        </is>
-      </c>
-      <c r="K3" t="inlineStr">
-        <is>
-          <t>15</t>
-        </is>
-      </c>
-      <c r="L3" t="inlineStr">
-        <is>
-          <t>15</t>
-        </is>
-      </c>
-      <c r="M3" t="inlineStr">
-        <is>
-          <t>30</t>
-        </is>
-      </c>
-    </row>
-    <row r="4">
-      <c r="A4" t="inlineStr">
-        <is>
-          <t>WALLE</t>
-        </is>
-      </c>
-      <c r="B4" t="inlineStr">
-        <is>
-          <t>comedy</t>
-        </is>
-      </c>
-      <c r="C4" t="inlineStr">
-        <is>
-          <t>120</t>
-        </is>
-      </c>
-      <c r="D4" t="inlineStr">
-        <is>
-          <t>robots</t>
-        </is>
-      </c>
-      <c r="E4" t="inlineStr">
-        <is>
-          <t>eva</t>
-        </is>
-      </c>
-      <c r="F4" t="inlineStr">
-        <is>
-          <t>5</t>
-        </is>
-      </c>
-      <c r="G4" t="inlineStr">
-        <is>
-          <t>English</t>
-        </is>
-      </c>
-      <c r="H4" t="inlineStr">
-        <is>
-          <t>03:00-05:00</t>
-        </is>
-      </c>
-      <c r="I4" t="inlineStr">
-        <is>
-          <t>3</t>
-        </is>
-      </c>
-      <c r="J4" t="inlineStr">
-        <is>
-          <t>8</t>
-        </is>
-      </c>
-      <c r="K4" t="inlineStr">
-        <is>
-          <t>15</t>
-        </is>
-      </c>
-      <c r="L4" t="inlineStr">
-        <is>
-          <t>15</t>
-        </is>
-      </c>
-      <c r="M4" t="inlineStr">
-        <is>
-          <t>30</t>
-        </is>
+      <c r="M4" t="n">
+        <v>100</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
This commit is to fix issues with cancel ticket
</commit_message>
<xml_diff>
--- a/DataSheet.xlsx
+++ b/DataSheet.xlsx
@@ -9,6 +9,7 @@
     <sheet name="Details" sheetId="1" state="visible" r:id="rId1"/>
     <sheet name="Pushpa" sheetId="2" state="visible" r:id="rId2"/>
     <sheet name="Krish" sheetId="3" state="visible" r:id="rId3"/>
+    <sheet name="walle" sheetId="4" state="visible" r:id="rId4"/>
   </sheets>
   <definedNames/>
   <calcPr calcId="0" fullCalcOnLoad="1"/>
@@ -426,7 +427,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:B7"/>
+  <dimension ref="A1:B8"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="D7" sqref="D7"/>
@@ -513,6 +514,18 @@
         </is>
       </c>
       <c r="B7" t="inlineStr">
+        <is>
+          <t>123</t>
+        </is>
+      </c>
+    </row>
+    <row r="8">
+      <c r="A8" t="inlineStr">
+        <is>
+          <t>ram</t>
+        </is>
+      </c>
+      <c r="B8" t="inlineStr">
         <is>
           <t>123</t>
         </is>
@@ -1097,4 +1110,299 @@
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <sheetPr>
+    <outlinePr summaryBelow="1" summaryRight="1"/>
+    <pageSetUpPr/>
+  </sheetPr>
+  <dimension ref="A1:N4"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A1" sqref="A1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
+  <sheetData>
+    <row r="1">
+      <c r="A1" t="inlineStr">
+        <is>
+          <t>title</t>
+        </is>
+      </c>
+      <c r="B1" t="inlineStr">
+        <is>
+          <t>genre</t>
+        </is>
+      </c>
+      <c r="C1" t="inlineStr">
+        <is>
+          <t>length</t>
+        </is>
+      </c>
+      <c r="D1" t="inlineStr">
+        <is>
+          <t>cast</t>
+        </is>
+      </c>
+      <c r="E1" t="inlineStr">
+        <is>
+          <t>director</t>
+        </is>
+      </c>
+      <c r="F1" t="inlineStr">
+        <is>
+          <t>rating</t>
+        </is>
+      </c>
+      <c r="G1" t="inlineStr">
+        <is>
+          <t>language</t>
+        </is>
+      </c>
+      <c r="H1" t="inlineStr">
+        <is>
+          <t>timings</t>
+        </is>
+      </c>
+      <c r="I1" t="inlineStr">
+        <is>
+          <t>shows_per_day</t>
+        </is>
+      </c>
+      <c r="J1" t="inlineStr">
+        <is>
+          <t>firstshow</t>
+        </is>
+      </c>
+      <c r="K1" t="inlineStr">
+        <is>
+          <t>interval_time</t>
+        </is>
+      </c>
+      <c r="L1" t="inlineStr">
+        <is>
+          <t>gap</t>
+        </is>
+      </c>
+      <c r="M1" t="inlineStr">
+        <is>
+          <t>capacity</t>
+        </is>
+      </c>
+      <c r="N1" t="inlineStr">
+        <is>
+          <t>user_count</t>
+        </is>
+      </c>
+    </row>
+    <row r="2">
+      <c r="A2" t="inlineStr">
+        <is>
+          <t>walle</t>
+        </is>
+      </c>
+      <c r="B2" t="inlineStr">
+        <is>
+          <t>comedy</t>
+        </is>
+      </c>
+      <c r="C2" t="inlineStr">
+        <is>
+          <t>120</t>
+        </is>
+      </c>
+      <c r="D2" t="inlineStr">
+        <is>
+          <t>w&amp;e</t>
+        </is>
+      </c>
+      <c r="E2" t="inlineStr">
+        <is>
+          <t>ani</t>
+        </is>
+      </c>
+      <c r="F2" t="inlineStr">
+        <is>
+          <t>5</t>
+        </is>
+      </c>
+      <c r="G2" t="inlineStr">
+        <is>
+          <t>eng</t>
+        </is>
+      </c>
+      <c r="H2" t="inlineStr">
+        <is>
+          <t>10:00-12:00</t>
+        </is>
+      </c>
+      <c r="I2" t="inlineStr">
+        <is>
+          <t>3</t>
+        </is>
+      </c>
+      <c r="J2" t="inlineStr">
+        <is>
+          <t>10</t>
+        </is>
+      </c>
+      <c r="K2" t="inlineStr">
+        <is>
+          <t>15</t>
+        </is>
+      </c>
+      <c r="L2" t="inlineStr">
+        <is>
+          <t>15</t>
+        </is>
+      </c>
+      <c r="M2" t="inlineStr">
+        <is>
+          <t>200</t>
+        </is>
+      </c>
+      <c r="N2" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="3">
+      <c r="A3" t="inlineStr">
+        <is>
+          <t>walle</t>
+        </is>
+      </c>
+      <c r="B3" t="inlineStr">
+        <is>
+          <t>comedy</t>
+        </is>
+      </c>
+      <c r="C3" t="inlineStr">
+        <is>
+          <t>120</t>
+        </is>
+      </c>
+      <c r="D3" t="inlineStr">
+        <is>
+          <t>w&amp;e</t>
+        </is>
+      </c>
+      <c r="E3" t="inlineStr">
+        <is>
+          <t>ani</t>
+        </is>
+      </c>
+      <c r="F3" t="inlineStr">
+        <is>
+          <t>5</t>
+        </is>
+      </c>
+      <c r="G3" t="inlineStr">
+        <is>
+          <t>eng</t>
+        </is>
+      </c>
+      <c r="H3" t="inlineStr">
+        <is>
+          <t>12:30-02:30</t>
+        </is>
+      </c>
+      <c r="I3" t="inlineStr">
+        <is>
+          <t>3</t>
+        </is>
+      </c>
+      <c r="J3" t="inlineStr">
+        <is>
+          <t>10</t>
+        </is>
+      </c>
+      <c r="K3" t="inlineStr">
+        <is>
+          <t>15</t>
+        </is>
+      </c>
+      <c r="L3" t="inlineStr">
+        <is>
+          <t>15</t>
+        </is>
+      </c>
+      <c r="M3" t="inlineStr">
+        <is>
+          <t>200</t>
+        </is>
+      </c>
+    </row>
+    <row r="4">
+      <c r="A4" t="inlineStr">
+        <is>
+          <t>walle</t>
+        </is>
+      </c>
+      <c r="B4" t="inlineStr">
+        <is>
+          <t>comedy</t>
+        </is>
+      </c>
+      <c r="C4" t="inlineStr">
+        <is>
+          <t>120</t>
+        </is>
+      </c>
+      <c r="D4" t="inlineStr">
+        <is>
+          <t>w&amp;e</t>
+        </is>
+      </c>
+      <c r="E4" t="inlineStr">
+        <is>
+          <t>ani</t>
+        </is>
+      </c>
+      <c r="F4" t="inlineStr">
+        <is>
+          <t>5</t>
+        </is>
+      </c>
+      <c r="G4" t="inlineStr">
+        <is>
+          <t>eng</t>
+        </is>
+      </c>
+      <c r="H4" t="inlineStr">
+        <is>
+          <t>03:00-05:00</t>
+        </is>
+      </c>
+      <c r="I4" t="inlineStr">
+        <is>
+          <t>3</t>
+        </is>
+      </c>
+      <c r="J4" t="inlineStr">
+        <is>
+          <t>10</t>
+        </is>
+      </c>
+      <c r="K4" t="inlineStr">
+        <is>
+          <t>15</t>
+        </is>
+      </c>
+      <c r="L4" t="inlineStr">
+        <is>
+          <t>15</t>
+        </is>
+      </c>
+      <c r="M4" t="inlineStr">
+        <is>
+          <t>200</t>
+        </is>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+</worksheet>
 </file>
</xml_diff>